<commit_message>
add drone survey data
</commit_message>
<xml_diff>
--- a/Data/taxa/CorrectedTaxonList.xlsx
+++ b/Data/taxa/CorrectedTaxonList.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mawha\Dropbox\Martone Lab\martone_calvert\Data\taxa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC47828B-686D-4784-AB1C-435DB635E068}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AD4BA6-271C-46B3-9C1C-E3688762A680}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3915" yWindow="465" windowWidth="24960" windowHeight="14025" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Change log" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="577">
   <si>
     <t>taxon</t>
   </si>
@@ -1608,9 +1609,6 @@
     <t>Littorina sp.</t>
   </si>
   <si>
-    <t>Lophopanopeus bellusopeus</t>
-  </si>
-  <si>
     <t>Lottia sp.</t>
   </si>
   <si>
@@ -1738,13 +1736,34 @@
   </si>
   <si>
     <t>kingdom</t>
+  </si>
+  <si>
+    <t>by</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>Whalen</t>
+  </si>
+  <si>
+    <t>change species name for Lophopanopeus</t>
+  </si>
+  <si>
+    <t>Lophopanopeus bellus</t>
+  </si>
+  <si>
+    <t>bare rock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1752,8 +1771,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1778,6 +1805,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1791,12 +1824,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2079,8 +2113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F464"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2100,10 +2134,10 @@
         <v>508</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E1" t="s">
         <v>22</v>
@@ -2135,7 +2169,7 @@
       </c>
       <c r="C3"/>
       <c r="D3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
@@ -2150,7 +2184,7 @@
       </c>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
@@ -2165,7 +2199,7 @@
       </c>
       <c r="C5"/>
       <c r="D5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
@@ -2179,7 +2213,7 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E6" t="s">
         <v>22</v>
@@ -2194,7 +2228,7 @@
       </c>
       <c r="C7"/>
       <c r="D7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
@@ -2205,10 +2239,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D8" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
@@ -2223,7 +2257,7 @@
       </c>
       <c r="C9"/>
       <c r="D9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E9" t="s">
         <v>22</v>
@@ -2238,7 +2272,7 @@
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E10" t="s">
         <v>22</v>
@@ -2253,7 +2287,7 @@
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>
@@ -2310,7 +2344,7 @@
       </c>
       <c r="C15"/>
       <c r="D15" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
@@ -2451,7 +2485,7 @@
       </c>
       <c r="C25"/>
       <c r="D25" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E25" t="s">
         <v>22</v>
@@ -2466,7 +2500,7 @@
       </c>
       <c r="C26"/>
       <c r="D26" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E26" t="s">
         <v>22</v>
@@ -2509,7 +2543,7 @@
       </c>
       <c r="C29"/>
       <c r="D29" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E29" t="s">
         <v>22</v>
@@ -2524,7 +2558,7 @@
       </c>
       <c r="C30"/>
       <c r="D30" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E30" t="s">
         <v>22</v>
@@ -2535,13 +2569,13 @@
         <v>38</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>38</v>
+        <v>576</v>
       </c>
       <c r="D31" t="s">
         <v>39</v>
       </c>
       <c r="E31" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2549,13 +2583,13 @@
         <v>40</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>38</v>
+        <v>576</v>
       </c>
       <c r="D32" t="s">
         <v>39</v>
       </c>
       <c r="E32" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2563,13 +2597,13 @@
         <v>41</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>38</v>
+        <v>576</v>
       </c>
       <c r="D33" t="s">
         <v>39</v>
       </c>
       <c r="E33" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2577,13 +2611,13 @@
         <v>42</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>38</v>
+        <v>576</v>
       </c>
       <c r="D34" t="s">
         <v>39</v>
       </c>
       <c r="E34" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2591,13 +2625,13 @@
         <v>43</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>38</v>
+        <v>576</v>
       </c>
       <c r="D35" t="s">
         <v>39</v>
       </c>
       <c r="E35" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2665,7 +2699,7 @@
       </c>
       <c r="C40" s="1"/>
       <c r="D40" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E40" t="s">
         <v>22</v>
@@ -2679,7 +2713,7 @@
         <v>52</v>
       </c>
       <c r="D41" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E41" t="s">
         <v>22</v>
@@ -2693,7 +2727,7 @@
         <v>54</v>
       </c>
       <c r="D42" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E42" t="s">
         <v>22</v>
@@ -2707,7 +2741,7 @@
         <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E43" t="s">
         <v>22</v>
@@ -2721,7 +2755,7 @@
         <v>60</v>
       </c>
       <c r="D44" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E44" t="s">
         <v>22</v>
@@ -2735,7 +2769,7 @@
         <v>61</v>
       </c>
       <c r="D45" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E45" t="s">
         <v>22</v>
@@ -2749,7 +2783,7 @@
         <v>62</v>
       </c>
       <c r="D46" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E46" t="s">
         <v>22</v>
@@ -2763,7 +2797,7 @@
         <v>63</v>
       </c>
       <c r="D47" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E47" t="s">
         <v>22</v>
@@ -2777,7 +2811,7 @@
         <v>57</v>
       </c>
       <c r="D48" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E48" t="s">
         <v>22</v>
@@ -2794,7 +2828,7 @@
         <v>57</v>
       </c>
       <c r="D49" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E49" t="s">
         <v>22</v>
@@ -2808,7 +2842,7 @@
         <v>57</v>
       </c>
       <c r="D50" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E50" t="s">
         <v>22</v>
@@ -2822,7 +2856,7 @@
         <v>67</v>
       </c>
       <c r="D51" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E51" t="s">
         <v>22</v>
@@ -2836,7 +2870,7 @@
         <v>68</v>
       </c>
       <c r="D52" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E52" t="s">
         <v>22</v>
@@ -2850,7 +2884,7 @@
         <v>69</v>
       </c>
       <c r="D53" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E53" t="s">
         <v>22</v>
@@ -2864,7 +2898,7 @@
         <v>70</v>
       </c>
       <c r="D54" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E54" t="s">
         <v>22</v>
@@ -2878,7 +2912,7 @@
         <v>73</v>
       </c>
       <c r="D55" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E55" t="s">
         <v>22</v>
@@ -2892,7 +2926,7 @@
         <v>73</v>
       </c>
       <c r="D56" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E56" t="s">
         <v>22</v>
@@ -2906,7 +2940,7 @@
         <v>76</v>
       </c>
       <c r="D57" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E57" t="s">
         <v>22</v>
@@ -2920,7 +2954,7 @@
         <v>77</v>
       </c>
       <c r="D58" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E58" t="s">
         <v>22</v>
@@ -2931,10 +2965,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D59" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E59" t="s">
         <v>22</v>
@@ -2945,10 +2979,10 @@
         <v>72</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D60" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E60" t="s">
         <v>22</v>
@@ -2959,10 +2993,10 @@
         <v>390</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D61" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E61" t="s">
         <v>22</v>
@@ -2976,7 +3010,7 @@
         <v>78</v>
       </c>
       <c r="D62" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E62" t="s">
         <v>22</v>
@@ -2990,7 +3024,7 @@
         <v>78</v>
       </c>
       <c r="D63" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E63" t="s">
         <v>22</v>
@@ -3004,7 +3038,7 @@
         <v>80</v>
       </c>
       <c r="D64" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E64" t="s">
         <v>22</v>
@@ -3018,7 +3052,7 @@
         <v>64</v>
       </c>
       <c r="D65" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E65" t="s">
         <v>22</v>
@@ -3032,7 +3066,7 @@
         <v>64</v>
       </c>
       <c r="D66" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E66" t="s">
         <v>22</v>
@@ -3060,7 +3094,7 @@
         <v>83</v>
       </c>
       <c r="D68" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E68" t="s">
         <v>22</v>
@@ -3131,7 +3165,7 @@
       </c>
       <c r="C73"/>
       <c r="D73" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E73" t="s">
         <v>22</v>
@@ -3160,7 +3194,7 @@
       </c>
       <c r="C75"/>
       <c r="D75" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E75" t="s">
         <v>22</v>
@@ -3175,7 +3209,7 @@
       </c>
       <c r="C76"/>
       <c r="D76" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E76" t="s">
         <v>22</v>
@@ -3190,7 +3224,7 @@
       </c>
       <c r="C77"/>
       <c r="D77" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E77" t="s">
         <v>22</v>
@@ -3205,7 +3239,7 @@
       </c>
       <c r="C78"/>
       <c r="D78" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E78" t="s">
         <v>22</v>
@@ -3220,7 +3254,7 @@
       </c>
       <c r="C79"/>
       <c r="D79" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E79" t="s">
         <v>22</v>
@@ -3235,7 +3269,7 @@
       </c>
       <c r="C80"/>
       <c r="D80" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E80" t="s">
         <v>22</v>
@@ -3250,7 +3284,7 @@
       </c>
       <c r="C81"/>
       <c r="D81" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E81" t="s">
         <v>22</v>
@@ -3265,7 +3299,7 @@
       </c>
       <c r="C82"/>
       <c r="D82" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E82" t="s">
         <v>22</v>
@@ -3420,7 +3454,7 @@
       </c>
       <c r="C93"/>
       <c r="D93" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E93" t="s">
         <v>22</v>
@@ -3435,7 +3469,7 @@
       </c>
       <c r="C94"/>
       <c r="D94" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E94" t="s">
         <v>22</v>
@@ -3450,7 +3484,7 @@
       </c>
       <c r="C95"/>
       <c r="D95" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E95" t="s">
         <v>22</v>
@@ -3495,7 +3529,7 @@
         <v>39</v>
       </c>
       <c r="E98" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3507,7 +3541,7 @@
       </c>
       <c r="C99"/>
       <c r="D99" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E99" t="s">
         <v>22</v>
@@ -3522,7 +3556,7 @@
       </c>
       <c r="C100"/>
       <c r="D100" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E100" t="s">
         <v>22</v>
@@ -3537,7 +3571,7 @@
       </c>
       <c r="C101"/>
       <c r="D101" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E101" t="s">
         <v>22</v>
@@ -3552,7 +3586,7 @@
       </c>
       <c r="C102"/>
       <c r="D102" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E102" t="s">
         <v>22</v>
@@ -3567,7 +3601,7 @@
       </c>
       <c r="C103"/>
       <c r="D103" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E103" t="s">
         <v>22</v>
@@ -3578,11 +3612,11 @@
         <v>153</v>
       </c>
       <c r="B104" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C104"/>
       <c r="D104" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E104" t="s">
         <v>22</v>
@@ -3597,7 +3631,7 @@
       </c>
       <c r="C105"/>
       <c r="D105" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E105" t="s">
         <v>22</v>
@@ -3612,7 +3646,7 @@
       </c>
       <c r="C106"/>
       <c r="D106" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E106" t="s">
         <v>22</v>
@@ -3630,7 +3664,7 @@
       </c>
       <c r="C107"/>
       <c r="D107" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E107" t="s">
         <v>22</v>
@@ -3645,7 +3679,7 @@
       </c>
       <c r="C108"/>
       <c r="D108" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E108" t="s">
         <v>22</v>
@@ -3660,7 +3694,7 @@
       </c>
       <c r="C109"/>
       <c r="D109" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E109" t="s">
         <v>22</v>
@@ -3675,7 +3709,7 @@
       </c>
       <c r="C110"/>
       <c r="D110" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E110" t="s">
         <v>22</v>
@@ -3690,7 +3724,7 @@
       </c>
       <c r="C111"/>
       <c r="D111" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E111" t="s">
         <v>22</v>
@@ -3705,7 +3739,7 @@
       </c>
       <c r="C112"/>
       <c r="D112" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E112" t="s">
         <v>22</v>
@@ -3720,7 +3754,7 @@
       </c>
       <c r="C113"/>
       <c r="D113" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E113" t="s">
         <v>22</v>
@@ -3735,7 +3769,7 @@
       </c>
       <c r="C114"/>
       <c r="D114" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E114" t="s">
         <v>22</v>
@@ -3750,7 +3784,7 @@
       </c>
       <c r="C115"/>
       <c r="D115" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E115" t="s">
         <v>22</v>
@@ -3765,7 +3799,7 @@
       </c>
       <c r="C116"/>
       <c r="D116" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E116" t="s">
         <v>22</v>
@@ -3780,7 +3814,7 @@
       </c>
       <c r="C117"/>
       <c r="D117" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E117" t="s">
         <v>22</v>
@@ -3795,7 +3829,7 @@
       </c>
       <c r="C118"/>
       <c r="D118" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E118" t="s">
         <v>22</v>
@@ -3810,7 +3844,7 @@
       </c>
       <c r="C119"/>
       <c r="D119" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E119" t="s">
         <v>22</v>
@@ -3821,11 +3855,11 @@
         <v>128</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C120" s="1"/>
       <c r="D120" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E120" t="s">
         <v>22</v>
@@ -3836,11 +3870,11 @@
         <v>140</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E121" t="s">
         <v>22</v>
@@ -3851,11 +3885,11 @@
         <v>164</v>
       </c>
       <c r="B122" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C122"/>
       <c r="D122" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E122" t="s">
         <v>22</v>
@@ -3866,11 +3900,11 @@
         <v>165</v>
       </c>
       <c r="B123" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C123"/>
       <c r="D123" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E123" t="s">
         <v>22</v>
@@ -3881,11 +3915,11 @@
         <v>166</v>
       </c>
       <c r="B124" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C124"/>
       <c r="D124" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E124" t="s">
         <v>22</v>
@@ -3896,11 +3930,11 @@
         <v>495</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C125" s="1"/>
       <c r="D125" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E125" t="s">
         <v>22</v>
@@ -3915,7 +3949,7 @@
       </c>
       <c r="C126"/>
       <c r="D126" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E126" t="s">
         <v>22</v>
@@ -3926,7 +3960,7 @@
         <v>450</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D127" t="s">
         <v>3</v>
@@ -3940,7 +3974,7 @@
         <v>475</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D128" t="s">
         <v>3</v>
@@ -3972,7 +4006,7 @@
       </c>
       <c r="C130"/>
       <c r="D130" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E130" t="s">
         <v>22</v>
@@ -3987,7 +4021,7 @@
       </c>
       <c r="C131"/>
       <c r="D131" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E131" t="s">
         <v>22</v>
@@ -4016,7 +4050,7 @@
       </c>
       <c r="C133"/>
       <c r="D133" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E133" t="s">
         <v>22</v>
@@ -4027,7 +4061,7 @@
         <v>317</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D134" t="s">
         <v>3</v>
@@ -4048,7 +4082,7 @@
       </c>
       <c r="C135"/>
       <c r="D135" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E135" t="s">
         <v>22</v>
@@ -4063,7 +4097,7 @@
       </c>
       <c r="C136"/>
       <c r="D136" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E136" t="s">
         <v>22</v>
@@ -4092,7 +4126,7 @@
       </c>
       <c r="C138"/>
       <c r="D138" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E138" t="s">
         <v>22</v>
@@ -4107,7 +4141,7 @@
       </c>
       <c r="C139"/>
       <c r="D139" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E139" t="s">
         <v>22</v>
@@ -4122,7 +4156,7 @@
       </c>
       <c r="C140"/>
       <c r="D140" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E140" t="s">
         <v>22</v>
@@ -4137,7 +4171,7 @@
       </c>
       <c r="C141"/>
       <c r="D141" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E141" t="s">
         <v>22</v>
@@ -4152,7 +4186,7 @@
       </c>
       <c r="C142"/>
       <c r="D142" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E142" t="s">
         <v>22</v>
@@ -4167,7 +4201,7 @@
       </c>
       <c r="C143"/>
       <c r="D143" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E143" t="s">
         <v>22</v>
@@ -4182,7 +4216,7 @@
       </c>
       <c r="C144"/>
       <c r="D144" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E144" t="s">
         <v>22</v>
@@ -4197,7 +4231,7 @@
       </c>
       <c r="C145"/>
       <c r="D145" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E145" t="s">
         <v>22</v>
@@ -4208,11 +4242,11 @@
         <v>158</v>
       </c>
       <c r="B146" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C146"/>
       <c r="D146" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E146" t="s">
         <v>22</v>
@@ -4227,7 +4261,7 @@
       </c>
       <c r="C147"/>
       <c r="D147" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E147" t="s">
         <v>22</v>
@@ -4242,7 +4276,7 @@
       </c>
       <c r="C148"/>
       <c r="D148" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E148" t="s">
         <v>22</v>
@@ -4257,7 +4291,7 @@
       </c>
       <c r="C149"/>
       <c r="D149" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E149" t="s">
         <v>22</v>
@@ -4272,7 +4306,7 @@
       </c>
       <c r="C150"/>
       <c r="D150" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E150" t="s">
         <v>22</v>
@@ -4287,7 +4321,7 @@
       </c>
       <c r="C151"/>
       <c r="D151" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E151" t="s">
         <v>22</v>
@@ -4302,7 +4336,7 @@
       </c>
       <c r="C152"/>
       <c r="D152" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E152" t="s">
         <v>22</v>
@@ -4334,7 +4368,7 @@
       </c>
       <c r="C154"/>
       <c r="D154" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E154" t="s">
         <v>22</v>
@@ -4391,7 +4425,7 @@
       </c>
       <c r="C158"/>
       <c r="D158" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E158" t="s">
         <v>22</v>
@@ -4406,7 +4440,7 @@
       </c>
       <c r="C159"/>
       <c r="D159" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E159" t="s">
         <v>22</v>
@@ -4421,7 +4455,7 @@
       </c>
       <c r="C160"/>
       <c r="D160" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E160" t="s">
         <v>22</v>
@@ -4453,7 +4487,7 @@
       </c>
       <c r="C162"/>
       <c r="D162" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E162" t="s">
         <v>22</v>
@@ -4468,7 +4502,7 @@
       </c>
       <c r="C163"/>
       <c r="D163" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E163" t="s">
         <v>22</v>
@@ -4514,7 +4548,7 @@
       </c>
       <c r="C166"/>
       <c r="D166" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E166" t="s">
         <v>22</v>
@@ -4574,7 +4608,7 @@
       </c>
       <c r="C170"/>
       <c r="D170" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E170" t="s">
         <v>22</v>
@@ -4699,7 +4733,7 @@
       </c>
       <c r="C178"/>
       <c r="D178" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E178" t="s">
         <v>22</v>
@@ -4717,7 +4751,7 @@
       </c>
       <c r="C179"/>
       <c r="D179" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E179" t="s">
         <v>22</v>
@@ -4735,7 +4769,7 @@
       </c>
       <c r="C180" s="1"/>
       <c r="D180" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E180" t="s">
         <v>22</v>
@@ -4753,7 +4787,7 @@
       </c>
       <c r="C181"/>
       <c r="D181" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E181" t="s">
         <v>22</v>
@@ -4768,7 +4802,7 @@
       </c>
       <c r="C182"/>
       <c r="D182" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E182" t="s">
         <v>22</v>
@@ -4783,7 +4817,7 @@
       </c>
       <c r="C183"/>
       <c r="D183" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E183" t="s">
         <v>22</v>
@@ -4798,7 +4832,7 @@
       </c>
       <c r="C184"/>
       <c r="D184" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E184" t="s">
         <v>22</v>
@@ -4816,7 +4850,7 @@
       </c>
       <c r="C185"/>
       <c r="D185" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E185" t="s">
         <v>22</v>
@@ -4862,7 +4896,7 @@
       </c>
       <c r="C188"/>
       <c r="D188" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E188" t="s">
         <v>22</v>
@@ -4877,7 +4911,7 @@
       </c>
       <c r="C189"/>
       <c r="D189" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E189" t="s">
         <v>22</v>
@@ -4892,7 +4926,7 @@
       </c>
       <c r="C190"/>
       <c r="D190" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E190" t="s">
         <v>22</v>
@@ -4910,7 +4944,7 @@
       </c>
       <c r="C191"/>
       <c r="D191" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E191" t="s">
         <v>22</v>
@@ -4928,7 +4962,7 @@
       </c>
       <c r="C192"/>
       <c r="D192" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E192" t="s">
         <v>22</v>
@@ -4943,7 +4977,7 @@
       </c>
       <c r="C193"/>
       <c r="D193" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E193" t="s">
         <v>22</v>
@@ -4961,7 +4995,7 @@
       </c>
       <c r="C194"/>
       <c r="D194" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E194" t="s">
         <v>22</v>
@@ -4976,7 +5010,7 @@
       </c>
       <c r="C195"/>
       <c r="D195" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E195" t="s">
         <v>22</v>
@@ -4991,7 +5025,7 @@
       </c>
       <c r="C196"/>
       <c r="D196" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E196" t="s">
         <v>22</v>
@@ -5037,7 +5071,7 @@
       </c>
       <c r="C199"/>
       <c r="D199" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E199" t="s">
         <v>22</v>
@@ -5086,7 +5120,7 @@
       </c>
       <c r="C202"/>
       <c r="D202" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E202" t="s">
         <v>22</v>
@@ -5115,7 +5149,7 @@
       </c>
       <c r="C204"/>
       <c r="D204" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E204" t="s">
         <v>22</v>
@@ -5130,7 +5164,7 @@
       </c>
       <c r="C205"/>
       <c r="D205" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E205" t="s">
         <v>22</v>
@@ -5145,7 +5179,7 @@
       </c>
       <c r="C206"/>
       <c r="D206" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E206" t="s">
         <v>22</v>
@@ -5188,7 +5222,7 @@
       </c>
       <c r="C209"/>
       <c r="D209" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E209" t="s">
         <v>22</v>
@@ -5203,7 +5237,7 @@
       </c>
       <c r="C210"/>
       <c r="D210" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E210" t="s">
         <v>22</v>
@@ -5246,7 +5280,7 @@
       </c>
       <c r="C213"/>
       <c r="D213" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E213" t="s">
         <v>22</v>
@@ -5261,7 +5295,7 @@
       </c>
       <c r="C214"/>
       <c r="D214" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E214" t="s">
         <v>22</v>
@@ -5278,7 +5312,7 @@
         <v>236</v>
       </c>
       <c r="D215" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E215" t="s">
         <v>22</v>
@@ -5295,7 +5329,7 @@
         <v>236</v>
       </c>
       <c r="D216" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E216" t="s">
         <v>22</v>
@@ -5312,7 +5346,7 @@
         <v>237</v>
       </c>
       <c r="D217" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E217" t="s">
         <v>22</v>
@@ -5326,7 +5360,7 @@
         <v>237</v>
       </c>
       <c r="D218" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E218" t="s">
         <v>22</v>
@@ -5340,10 +5374,10 @@
         <v>240</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D219" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E219" t="s">
         <v>22</v>
@@ -5358,7 +5392,7 @@
       </c>
       <c r="C220"/>
       <c r="D220" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E220" t="s">
         <v>22</v>
@@ -5373,7 +5407,7 @@
       </c>
       <c r="C221"/>
       <c r="D221" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E221" t="s">
         <v>22</v>
@@ -5388,7 +5422,7 @@
       </c>
       <c r="C222"/>
       <c r="D222" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E222" t="s">
         <v>22</v>
@@ -5462,7 +5496,7 @@
       </c>
       <c r="C227"/>
       <c r="D227" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E227" t="s">
         <v>22</v>
@@ -5473,7 +5507,7 @@
         <v>249</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>527</v>
+        <v>575</v>
       </c>
       <c r="D228" t="s">
         <v>3</v>
@@ -5487,7 +5521,7 @@
         <v>250</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D229" t="s">
         <v>3</v>
@@ -5501,7 +5535,7 @@
         <v>251</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D230" t="s">
         <v>3</v>
@@ -5519,7 +5553,7 @@
       </c>
       <c r="C231"/>
       <c r="D231" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E231" t="s">
         <v>22</v>
@@ -5534,7 +5568,7 @@
       </c>
       <c r="C232"/>
       <c r="D232" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E232" t="s">
         <v>22</v>
@@ -5552,7 +5586,7 @@
       </c>
       <c r="C233"/>
       <c r="D233" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E233" t="s">
         <v>22</v>
@@ -5567,7 +5601,7 @@
       </c>
       <c r="C234"/>
       <c r="D234" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E234" t="s">
         <v>22</v>
@@ -5582,7 +5616,7 @@
       </c>
       <c r="C235"/>
       <c r="D235" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E235" t="s">
         <v>22</v>
@@ -5600,7 +5634,7 @@
       </c>
       <c r="C236"/>
       <c r="D236" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E236" t="s">
         <v>22</v>
@@ -5615,7 +5649,7 @@
       </c>
       <c r="C237"/>
       <c r="D237" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E237" t="s">
         <v>22</v>
@@ -5630,7 +5664,7 @@
       </c>
       <c r="C238"/>
       <c r="D238" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E238" t="s">
         <v>22</v>
@@ -5648,7 +5682,7 @@
       </c>
       <c r="C239"/>
       <c r="D239" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E239" t="s">
         <v>22</v>
@@ -5663,7 +5697,7 @@
       </c>
       <c r="C240"/>
       <c r="D240" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E240" t="s">
         <v>22</v>
@@ -5678,7 +5712,7 @@
       </c>
       <c r="C241"/>
       <c r="D241" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E241" t="s">
         <v>22</v>
@@ -5693,7 +5727,7 @@
       </c>
       <c r="C242"/>
       <c r="D242" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E242" t="s">
         <v>22</v>
@@ -5711,7 +5745,7 @@
       </c>
       <c r="C243"/>
       <c r="D243" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E243" t="s">
         <v>22</v>
@@ -5726,7 +5760,7 @@
       </c>
       <c r="C244"/>
       <c r="D244" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E244" t="s">
         <v>22</v>
@@ -5741,7 +5775,7 @@
       </c>
       <c r="C245"/>
       <c r="D245" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E245" t="s">
         <v>22</v>
@@ -5756,7 +5790,7 @@
       </c>
       <c r="C246"/>
       <c r="D246" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E246" t="s">
         <v>22</v>
@@ -5774,7 +5808,7 @@
       </c>
       <c r="C247"/>
       <c r="D247" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E247" t="s">
         <v>22</v>
@@ -5789,7 +5823,7 @@
       </c>
       <c r="C248"/>
       <c r="D248" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E248" t="s">
         <v>22</v>
@@ -5804,7 +5838,7 @@
       </c>
       <c r="C249"/>
       <c r="D249" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E249" t="s">
         <v>22</v>
@@ -5819,7 +5853,7 @@
       </c>
       <c r="C250"/>
       <c r="D250" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E250" t="s">
         <v>22</v>
@@ -5837,7 +5871,7 @@
       </c>
       <c r="C251"/>
       <c r="D251" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E251" t="s">
         <v>22</v>
@@ -5852,7 +5886,7 @@
       </c>
       <c r="C252"/>
       <c r="D252" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E252" t="s">
         <v>22</v>
@@ -5866,7 +5900,7 @@
         <v>432</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D253" t="s">
         <v>3</v>
@@ -5884,7 +5918,7 @@
       </c>
       <c r="C254"/>
       <c r="D254" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E254" t="s">
         <v>22</v>
@@ -5899,7 +5933,7 @@
       </c>
       <c r="C255"/>
       <c r="D255" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E255" t="s">
         <v>22</v>
@@ -5914,7 +5948,7 @@
       </c>
       <c r="C256"/>
       <c r="D256" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E256" t="s">
         <v>22</v>
@@ -5925,7 +5959,7 @@
         <v>282</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D257" t="s">
         <v>3</v>
@@ -5953,7 +5987,7 @@
         <v>283</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D259" t="s">
         <v>3</v>
@@ -5970,7 +6004,7 @@
         <v>285</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D260" t="s">
         <v>3</v>
@@ -5987,7 +6021,7 @@
         <v>286</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D261" t="s">
         <v>3</v>
@@ -6022,7 +6056,7 @@
       </c>
       <c r="C263"/>
       <c r="D263" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E263" t="s">
         <v>22</v>
@@ -6037,7 +6071,7 @@
       </c>
       <c r="C264"/>
       <c r="D264" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E264" t="s">
         <v>22</v>
@@ -6048,7 +6082,7 @@
         <v>291</v>
       </c>
       <c r="B265" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D265" t="s">
         <v>3</v>
@@ -6062,7 +6096,7 @@
         <v>292</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D266" t="s">
         <v>3</v>
@@ -6076,11 +6110,11 @@
         <v>13</v>
       </c>
       <c r="B267" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C267"/>
       <c r="D267" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E267" t="s">
         <v>22</v>
@@ -6095,7 +6129,7 @@
       </c>
       <c r="C268"/>
       <c r="D268" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E268" t="s">
         <v>22</v>
@@ -6110,7 +6144,7 @@
       </c>
       <c r="C269"/>
       <c r="D269" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E269" t="s">
         <v>22</v>
@@ -6128,7 +6162,7 @@
       </c>
       <c r="C270"/>
       <c r="D270" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E270" t="s">
         <v>22</v>
@@ -6143,7 +6177,7 @@
       </c>
       <c r="C271"/>
       <c r="D271" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E271" t="s">
         <v>22</v>
@@ -6158,7 +6192,7 @@
       </c>
       <c r="C272"/>
       <c r="D272" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E272" t="s">
         <v>22</v>
@@ -6173,7 +6207,7 @@
       </c>
       <c r="C273"/>
       <c r="D273" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E273" t="s">
         <v>22</v>
@@ -6188,7 +6222,7 @@
       </c>
       <c r="C274"/>
       <c r="D274" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E274" t="s">
         <v>22</v>
@@ -6203,7 +6237,7 @@
       </c>
       <c r="C275"/>
       <c r="D275" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E275" t="s">
         <v>22</v>
@@ -6221,7 +6255,7 @@
       </c>
       <c r="C276"/>
       <c r="D276" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E276" t="s">
         <v>22</v>
@@ -6236,7 +6270,7 @@
       </c>
       <c r="C277"/>
       <c r="D277" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E277" t="s">
         <v>22</v>
@@ -6251,7 +6285,7 @@
       </c>
       <c r="C278"/>
       <c r="D278" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E278" t="s">
         <v>22</v>
@@ -6262,7 +6296,7 @@
         <v>301</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D279" t="s">
         <v>3</v>
@@ -6283,7 +6317,7 @@
       </c>
       <c r="C280"/>
       <c r="D280" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E280" t="s">
         <v>22</v>
@@ -6342,7 +6376,7 @@
         <v>310</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D284" t="s">
         <v>3</v>
@@ -6363,7 +6397,7 @@
       </c>
       <c r="C285"/>
       <c r="D285" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E285" t="s">
         <v>22</v>
@@ -6381,7 +6415,7 @@
       </c>
       <c r="C286"/>
       <c r="D286" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E286" t="s">
         <v>22</v>
@@ -6409,7 +6443,7 @@
         <v>314</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D288" t="s">
         <v>3</v>
@@ -6427,7 +6461,7 @@
       </c>
       <c r="C289"/>
       <c r="D289" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E289" t="s">
         <v>22</v>
@@ -6442,7 +6476,7 @@
       </c>
       <c r="C290"/>
       <c r="D290" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E290" t="s">
         <v>22</v>
@@ -6516,7 +6550,7 @@
       </c>
       <c r="C295"/>
       <c r="D295" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E295" t="s">
         <v>22</v>
@@ -6534,7 +6568,7 @@
       </c>
       <c r="C296"/>
       <c r="D296" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E296" t="s">
         <v>22</v>
@@ -6586,7 +6620,7 @@
       </c>
       <c r="C299"/>
       <c r="D299" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E299" t="s">
         <v>22</v>
@@ -6604,7 +6638,7 @@
       </c>
       <c r="C300"/>
       <c r="D300" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E300" t="s">
         <v>22</v>
@@ -6622,7 +6656,7 @@
       </c>
       <c r="C301"/>
       <c r="D301" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E301" t="s">
         <v>22</v>
@@ -6637,7 +6671,7 @@
       </c>
       <c r="C302"/>
       <c r="D302" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E302" t="s">
         <v>22</v>
@@ -6655,7 +6689,7 @@
       </c>
       <c r="C303"/>
       <c r="D303" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E303" t="s">
         <v>22</v>
@@ -6670,7 +6704,7 @@
       </c>
       <c r="C304"/>
       <c r="D304" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E304" t="s">
         <v>22</v>
@@ -6685,7 +6719,7 @@
       </c>
       <c r="C305"/>
       <c r="D305" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E305" t="s">
         <v>22</v>
@@ -6714,7 +6748,7 @@
       </c>
       <c r="C307"/>
       <c r="D307" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E307" t="s">
         <v>22</v>
@@ -6729,7 +6763,7 @@
       </c>
       <c r="C308"/>
       <c r="D308" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E308" t="s">
         <v>22</v>
@@ -6744,7 +6778,7 @@
       </c>
       <c r="C309"/>
       <c r="D309" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E309" t="s">
         <v>22</v>
@@ -6759,7 +6793,7 @@
       </c>
       <c r="C310"/>
       <c r="D310" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E310" t="s">
         <v>22</v>
@@ -6770,11 +6804,11 @@
         <v>343</v>
       </c>
       <c r="B311" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C311"/>
       <c r="D311" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E311" t="s">
         <v>22</v>
@@ -6857,7 +6891,7 @@
       </c>
       <c r="C316"/>
       <c r="D316" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E316" t="s">
         <v>22</v>
@@ -6875,7 +6909,7 @@
       </c>
       <c r="C317"/>
       <c r="D317" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E317" t="s">
         <v>22</v>
@@ -6893,7 +6927,7 @@
       </c>
       <c r="C318"/>
       <c r="D318" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E318" t="s">
         <v>22</v>
@@ -6904,7 +6938,7 @@
         <v>354</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D319" t="s">
         <v>3</v>
@@ -6978,7 +7012,7 @@
       </c>
       <c r="C324"/>
       <c r="D324" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E324" t="s">
         <v>22</v>
@@ -6996,7 +7030,7 @@
       </c>
       <c r="C325"/>
       <c r="D325" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E325" t="s">
         <v>22</v>
@@ -7014,7 +7048,7 @@
       </c>
       <c r="C326"/>
       <c r="D326" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E326" t="s">
         <v>22</v>
@@ -7032,7 +7066,7 @@
       </c>
       <c r="C327"/>
       <c r="D327" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E327" t="s">
         <v>22</v>
@@ -7047,7 +7081,7 @@
       </c>
       <c r="C328"/>
       <c r="D328" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E328" t="s">
         <v>22</v>
@@ -7062,7 +7096,7 @@
       </c>
       <c r="C329"/>
       <c r="D329" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E329" t="s">
         <v>22</v>
@@ -7077,7 +7111,7 @@
       </c>
       <c r="C330"/>
       <c r="D330" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E330" t="s">
         <v>22</v>
@@ -7095,7 +7129,7 @@
       </c>
       <c r="C331"/>
       <c r="D331" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E331" t="s">
         <v>22</v>
@@ -7110,7 +7144,7 @@
       </c>
       <c r="C332"/>
       <c r="D332" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E332" t="s">
         <v>22</v>
@@ -7125,7 +7159,7 @@
       </c>
       <c r="C333"/>
       <c r="D333" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E333" t="s">
         <v>22</v>
@@ -7143,7 +7177,7 @@
       </c>
       <c r="C334"/>
       <c r="D334" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E334" t="s">
         <v>22</v>
@@ -7158,7 +7192,7 @@
       </c>
       <c r="C335"/>
       <c r="D335" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E335" t="s">
         <v>22</v>
@@ -7176,7 +7210,7 @@
       </c>
       <c r="C336"/>
       <c r="D336" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E336" t="s">
         <v>22</v>
@@ -7191,7 +7225,7 @@
       </c>
       <c r="C337"/>
       <c r="D337" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E337" t="s">
         <v>22</v>
@@ -7206,7 +7240,7 @@
       </c>
       <c r="C338"/>
       <c r="D338" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E338" t="s">
         <v>22</v>
@@ -7221,7 +7255,7 @@
       </c>
       <c r="C339"/>
       <c r="D339" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E339" t="s">
         <v>22</v>
@@ -7235,7 +7269,7 @@
         <v>318</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D340" t="s">
         <v>3</v>
@@ -7249,7 +7283,7 @@
         <v>319</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D341" t="s">
         <v>3</v>
@@ -7266,7 +7300,7 @@
         <v>412</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D342" t="s">
         <v>3</v>
@@ -7283,7 +7317,7 @@
         <v>466</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D343" t="s">
         <v>3</v>
@@ -7300,7 +7334,7 @@
         <v>473</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D344" t="s">
         <v>3</v>
@@ -7314,7 +7348,7 @@
         <v>497</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D345" t="s">
         <v>3</v>
@@ -7331,11 +7365,11 @@
         <v>383</v>
       </c>
       <c r="B346" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C346"/>
       <c r="D346" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E346" t="s">
         <v>22</v>
@@ -7346,11 +7380,11 @@
         <v>384</v>
       </c>
       <c r="B347" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C347"/>
       <c r="D347" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E347" t="s">
         <v>22</v>
@@ -7365,7 +7399,7 @@
       </c>
       <c r="C348"/>
       <c r="D348" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E348" t="s">
         <v>22</v>
@@ -7379,7 +7413,7 @@
         <v>386</v>
       </c>
       <c r="D349" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E349" t="s">
         <v>22</v>
@@ -7393,7 +7427,7 @@
         <v>386</v>
       </c>
       <c r="D350" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E350" t="s">
         <v>22</v>
@@ -7411,7 +7445,7 @@
       </c>
       <c r="C351"/>
       <c r="D351" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E351" t="s">
         <v>22</v>
@@ -7426,7 +7460,7 @@
       </c>
       <c r="C352"/>
       <c r="D352" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E352" t="s">
         <v>22</v>
@@ -7444,7 +7478,7 @@
       </c>
       <c r="C353"/>
       <c r="D353" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E353" t="s">
         <v>22</v>
@@ -7462,7 +7496,7 @@
       </c>
       <c r="C354"/>
       <c r="D354" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E354" t="s">
         <v>22</v>
@@ -7480,7 +7514,7 @@
       </c>
       <c r="C355"/>
       <c r="D355" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E355" t="s">
         <v>22</v>
@@ -7498,7 +7532,7 @@
       </c>
       <c r="C356"/>
       <c r="D356" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E356" t="s">
         <v>22</v>
@@ -7512,11 +7546,11 @@
         <v>398</v>
       </c>
       <c r="B357" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C357"/>
       <c r="D357" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E357" t="s">
         <v>22</v>
@@ -7530,11 +7564,11 @@
         <v>399</v>
       </c>
       <c r="B358" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C358"/>
       <c r="D358" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E358" t="s">
         <v>22</v>
@@ -7552,7 +7586,7 @@
       </c>
       <c r="C359"/>
       <c r="D359" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E359" t="s">
         <v>22</v>
@@ -7567,7 +7601,7 @@
       </c>
       <c r="C360"/>
       <c r="D360" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E360" t="s">
         <v>22</v>
@@ -7582,7 +7616,7 @@
       </c>
       <c r="C361"/>
       <c r="D361" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E361" t="s">
         <v>22</v>
@@ -7597,7 +7631,7 @@
       </c>
       <c r="C362"/>
       <c r="D362" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E362" t="s">
         <v>22</v>
@@ -7612,7 +7646,7 @@
       </c>
       <c r="C363"/>
       <c r="D363" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E363" t="s">
         <v>22</v>
@@ -7654,7 +7688,7 @@
         <v>405</v>
       </c>
       <c r="B366" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D366" t="s">
         <v>407</v>
@@ -7672,7 +7706,7 @@
       </c>
       <c r="C367"/>
       <c r="D367" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E367" t="s">
         <v>22</v>
@@ -7690,7 +7724,7 @@
       </c>
       <c r="C368"/>
       <c r="D368" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E368" t="s">
         <v>22</v>
@@ -7704,7 +7738,7 @@
         <v>415</v>
       </c>
       <c r="B369" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D369" t="s">
         <v>3</v>
@@ -7725,7 +7759,7 @@
       </c>
       <c r="C370"/>
       <c r="D370" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E370" t="s">
         <v>22</v>
@@ -7743,7 +7777,7 @@
       </c>
       <c r="C371"/>
       <c r="D371" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E371" t="s">
         <v>22</v>
@@ -7761,7 +7795,7 @@
       </c>
       <c r="C372"/>
       <c r="D372" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E372" t="s">
         <v>22</v>
@@ -7779,7 +7813,7 @@
       </c>
       <c r="C373"/>
       <c r="D373" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E373" t="s">
         <v>22</v>
@@ -7797,7 +7831,7 @@
       </c>
       <c r="C374"/>
       <c r="D374" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E374" t="s">
         <v>22</v>
@@ -7815,7 +7849,7 @@
       </c>
       <c r="C375"/>
       <c r="D375" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E375" t="s">
         <v>22</v>
@@ -7833,7 +7867,7 @@
       </c>
       <c r="C376"/>
       <c r="D376" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E376" t="s">
         <v>22</v>
@@ -7851,7 +7885,7 @@
       </c>
       <c r="C377"/>
       <c r="D377" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E377" t="s">
         <v>22</v>
@@ -7869,7 +7903,7 @@
       </c>
       <c r="C378"/>
       <c r="D378" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E378" t="s">
         <v>22</v>
@@ -7887,7 +7921,7 @@
       </c>
       <c r="C379"/>
       <c r="D379" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E379" t="s">
         <v>22</v>
@@ -7905,7 +7939,7 @@
       </c>
       <c r="C380"/>
       <c r="D380" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E380" t="s">
         <v>22</v>
@@ -7923,7 +7957,7 @@
       </c>
       <c r="C381"/>
       <c r="D381" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E381" t="s">
         <v>22</v>
@@ -7937,11 +7971,11 @@
         <v>422</v>
       </c>
       <c r="B382" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C382"/>
       <c r="D382" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E382" t="s">
         <v>22</v>
@@ -7955,11 +7989,11 @@
         <v>424</v>
       </c>
       <c r="B383" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C383"/>
       <c r="D383" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E383" t="s">
         <v>22</v>
@@ -7973,17 +8007,17 @@
         <v>425</v>
       </c>
       <c r="B384" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C384"/>
       <c r="D384" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E384" t="s">
         <v>22</v>
       </c>
       <c r="F384" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="385" spans="1:6" x14ac:dyDescent="0.25">
@@ -7991,11 +8025,11 @@
         <v>426</v>
       </c>
       <c r="B385" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C385"/>
       <c r="D385" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E385" t="s">
         <v>22</v>
@@ -8009,11 +8043,11 @@
         <v>427</v>
       </c>
       <c r="B386" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C386"/>
       <c r="D386" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E386" t="s">
         <v>22</v>
@@ -8027,11 +8061,11 @@
         <v>428</v>
       </c>
       <c r="B387" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C387"/>
       <c r="D387" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E387" t="s">
         <v>22</v>
@@ -8045,11 +8079,11 @@
         <v>429</v>
       </c>
       <c r="B388" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C388"/>
       <c r="D388" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E388" t="s">
         <v>22</v>
@@ -8067,7 +8101,7 @@
       </c>
       <c r="C389"/>
       <c r="D389" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E389" t="s">
         <v>22</v>
@@ -8085,7 +8119,7 @@
       </c>
       <c r="C390"/>
       <c r="D390" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E390" t="s">
         <v>22</v>
@@ -8103,7 +8137,7 @@
       </c>
       <c r="C391"/>
       <c r="D391" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E391" t="s">
         <v>22</v>
@@ -8121,7 +8155,7 @@
       </c>
       <c r="C392"/>
       <c r="D392" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E392" t="s">
         <v>22</v>
@@ -8153,7 +8187,7 @@
       </c>
       <c r="C394"/>
       <c r="D394" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E394" t="s">
         <v>22</v>
@@ -8171,7 +8205,7 @@
       </c>
       <c r="C395"/>
       <c r="D395" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E395" t="s">
         <v>22</v>
@@ -8186,7 +8220,7 @@
       </c>
       <c r="C396"/>
       <c r="D396" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E396" t="s">
         <v>22</v>
@@ -8201,7 +8235,7 @@
       </c>
       <c r="C397"/>
       <c r="D397" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E397" t="s">
         <v>22</v>
@@ -8216,7 +8250,7 @@
       </c>
       <c r="C398"/>
       <c r="D398" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E398" t="s">
         <v>22</v>
@@ -8231,7 +8265,7 @@
       </c>
       <c r="C399"/>
       <c r="D399" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E399" t="s">
         <v>22</v>
@@ -8248,7 +8282,7 @@
         <v>39</v>
       </c>
       <c r="E400" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F400" t="s">
         <v>400</v>
@@ -8263,7 +8297,7 @@
       </c>
       <c r="C401"/>
       <c r="D401" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E401" t="s">
         <v>22</v>
@@ -8278,7 +8312,7 @@
       </c>
       <c r="C402"/>
       <c r="D402" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E402" t="s">
         <v>22</v>
@@ -8293,7 +8327,7 @@
       </c>
       <c r="C403"/>
       <c r="D403" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E403" t="s">
         <v>22</v>
@@ -8308,7 +8342,7 @@
       </c>
       <c r="C404"/>
       <c r="D404" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E404" t="s">
         <v>22</v>
@@ -8323,7 +8357,7 @@
       </c>
       <c r="C405"/>
       <c r="D405" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E405" t="s">
         <v>22</v>
@@ -8341,7 +8375,7 @@
       </c>
       <c r="C406"/>
       <c r="D406" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E406" t="s">
         <v>22</v>
@@ -8359,7 +8393,7 @@
       </c>
       <c r="C407"/>
       <c r="D407" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E407" t="s">
         <v>22</v>
@@ -8370,7 +8404,7 @@
         <v>454</v>
       </c>
       <c r="B408" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D408" t="s">
         <v>3</v>
@@ -8430,7 +8464,7 @@
       </c>
       <c r="C412"/>
       <c r="D412" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E412" t="s">
         <v>22</v>
@@ -8473,7 +8507,7 @@
       </c>
       <c r="C415"/>
       <c r="D415" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E415" t="s">
         <v>22</v>
@@ -8488,7 +8522,7 @@
       </c>
       <c r="C416"/>
       <c r="D416" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E416" t="s">
         <v>22</v>
@@ -8503,7 +8537,7 @@
       </c>
       <c r="C417"/>
       <c r="D417" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E417" t="s">
         <v>22</v>
@@ -8554,7 +8588,7 @@
         <v>388</v>
       </c>
       <c r="D420" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E420" t="s">
         <v>22</v>
@@ -8571,7 +8605,7 @@
         <v>388</v>
       </c>
       <c r="D421" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E421" t="s">
         <v>22</v>
@@ -8589,7 +8623,7 @@
       </c>
       <c r="C422"/>
       <c r="D422" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E422" t="s">
         <v>22</v>
@@ -8665,7 +8699,7 @@
         <v>470</v>
       </c>
       <c r="B427" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D427" t="s">
         <v>3</v>
@@ -8682,7 +8716,7 @@
         <v>471</v>
       </c>
       <c r="B428" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D428" t="s">
         <v>3</v>
@@ -8696,7 +8730,7 @@
         <v>474</v>
       </c>
       <c r="B429" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D429" t="s">
         <v>3</v>
@@ -8717,7 +8751,7 @@
       </c>
       <c r="C430"/>
       <c r="D430" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E430" t="s">
         <v>22</v>
@@ -8732,7 +8766,7 @@
       </c>
       <c r="C431"/>
       <c r="D431" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E431" t="s">
         <v>22</v>
@@ -8763,7 +8797,7 @@
         <v>478</v>
       </c>
       <c r="B433" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D433" t="s">
         <v>3</v>
@@ -8833,7 +8867,7 @@
         <v>167</v>
       </c>
       <c r="B438" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D438" t="s">
         <v>3</v>
@@ -8847,7 +8881,7 @@
         <v>320</v>
       </c>
       <c r="B439" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D439" t="s">
         <v>3</v>
@@ -8861,7 +8895,7 @@
         <v>467</v>
       </c>
       <c r="B440" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D440" t="s">
         <v>3</v>
@@ -8878,7 +8912,7 @@
         <v>483</v>
       </c>
       <c r="B441" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D441" t="s">
         <v>3</v>
@@ -8892,7 +8926,7 @@
         <v>498</v>
       </c>
       <c r="B442" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D442" t="s">
         <v>3</v>
@@ -8906,7 +8940,7 @@
         <v>484</v>
       </c>
       <c r="B443" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C443" s="1"/>
       <c r="D443" t="s">
@@ -8921,11 +8955,11 @@
         <v>485</v>
       </c>
       <c r="B444" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C444"/>
       <c r="D444" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E444" t="s">
         <v>22</v>
@@ -8940,7 +8974,7 @@
       </c>
       <c r="C445"/>
       <c r="D445" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E445" t="s">
         <v>22</v>
@@ -8955,7 +8989,7 @@
       </c>
       <c r="C446"/>
       <c r="D446" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E446" t="s">
         <v>22</v>
@@ -8973,7 +9007,7 @@
       </c>
       <c r="C447"/>
       <c r="D447" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E447" t="s">
         <v>22</v>
@@ -8988,7 +9022,7 @@
       </c>
       <c r="C448"/>
       <c r="D448" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E448" t="s">
         <v>22</v>
@@ -9003,7 +9037,7 @@
       </c>
       <c r="C449"/>
       <c r="D449" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E449" t="s">
         <v>22</v>
@@ -9018,7 +9052,7 @@
       </c>
       <c r="C450"/>
       <c r="D450" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E450" t="s">
         <v>22</v>
@@ -9029,11 +9063,11 @@
         <v>430</v>
       </c>
       <c r="B451" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C451" s="1"/>
       <c r="D451" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E451" t="s">
         <v>22</v>
@@ -9044,11 +9078,11 @@
         <v>493</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C452" s="1"/>
       <c r="D452" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E452" t="s">
         <v>22</v>
@@ -9059,11 +9093,11 @@
         <v>494</v>
       </c>
       <c r="B453" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C453" s="1"/>
       <c r="D453" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E453" t="s">
         <v>22</v>
@@ -9074,11 +9108,11 @@
         <v>499</v>
       </c>
       <c r="B454" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C454" s="1"/>
       <c r="D454" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E454" t="s">
         <v>22</v>
@@ -9089,11 +9123,11 @@
         <v>492</v>
       </c>
       <c r="B455" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C455" s="1"/>
       <c r="D455" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E455" t="s">
         <v>22</v>
@@ -9104,11 +9138,11 @@
         <v>502</v>
       </c>
       <c r="B456" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C456"/>
       <c r="D456" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E456" t="s">
         <v>22</v>
@@ -9119,11 +9153,11 @@
         <v>504</v>
       </c>
       <c r="B457" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C457"/>
       <c r="D457" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E457" t="s">
         <v>22</v>
@@ -9138,7 +9172,7 @@
       </c>
       <c r="C458"/>
       <c r="D458" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E458" t="s">
         <v>22</v>
@@ -9153,7 +9187,7 @@
       </c>
       <c r="C459"/>
       <c r="D459" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E459" t="s">
         <v>22</v>
@@ -9164,11 +9198,11 @@
         <v>379</v>
       </c>
       <c r="B460" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C460"/>
       <c r="D460" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E460" t="s">
         <v>22</v>
@@ -9179,13 +9213,13 @@
         <v>506</v>
       </c>
       <c r="B461" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D461" t="s">
         <v>39</v>
       </c>
       <c r="E461" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F461" t="s">
         <v>501</v>
@@ -9231,7 +9265,7 @@
       </c>
       <c r="B464" s="1"/>
       <c r="D464" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E464" t="s">
         <v>22</v>
@@ -9243,4 +9277,42 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF5CBD1F-5400-4D42-AA21-D41B4E370A1C}">
+  <dimension ref="A2:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20190129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>573</v>
+      </c>
+      <c r="C3" t="s">
+        <v>574</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>